<commit_message>
Eliminacion de time loop en procesamiento
Sigue presentandose el problema de desfasaje
</commit_message>
<xml_diff>
--- a/MedidorInteligente_V1/Valores de calibracion.xlsx
+++ b/MedidorInteligente_V1/Valores de calibracion.xlsx
@@ -422,7 +422,7 @@
   <dimension ref="A1:V18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+      <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -814,7 +814,7 @@
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
     </row>
-    <row r="16" spans="1:22" ht="30">
+    <row r="16" spans="1:22">
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>

</xml_diff>